<commit_message>
Performed annotation, added 2 missing gnds
</commit_message>
<xml_diff>
--- a/motor-control/maybe-bom.xlsx
+++ b/motor-control/maybe-bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="148">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>C21</t>
+  </si>
+  <si>
+    <t>"C:\Program Files\KiCad\bin\xsltproc.exe" -v -o motor-interface-rev1.csv "C:\Program Files\KiCad\bin\scripting\plugins\bom2csv.xsl" motor-interface-rev1.xml</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
   <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,6 +853,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>13</v>

</xml_diff>